<commit_message>
Test and examples added
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/002_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/002_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="Re7c0707ea69241ad"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="Rdab2dff271904f52"/>
   </x:sheets>
   <x:calcPr fullCalcOnLoad="1"/>
 </x:workbook>
@@ -97,7 +97,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>46038.74828180556</x:v>
+        <x:v>46039.691805138886</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -105,7 +105,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>46038.74828180556</x:v>
+        <x:v>46039.691805138886</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Font issues. Update OpenDoc
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/002_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/002_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="Rbfb1abde5fb04691"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R5a4589c6b6884ba8"/>
   </x:sheets>
   <x:calcPr fullCalcOnLoad="1"/>
 </x:workbook>
@@ -97,7 +97,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>46039.78580196759</x:v>
+        <x:v>46040.34884</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -105,7 +105,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>46039.78580196759</x:v>
+        <x:v>46040.34884</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
5.0.0 Added caching of typefaces due to performance issues.
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/002_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/002_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="Re5eebc6936ff42b0"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R8a6250edefca43e9"/>
   </x:sheets>
   <x:calcPr fullCalcOnLoad="1"/>
 </x:workbook>
@@ -97,7 +97,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>46040.94270907407</x:v>
+        <x:v>46040.98596686342</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -105,7 +105,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>46040.94270907407</x:v>
+        <x:v>46040.98596686342</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Cache fix and json export
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/002_DataTypes.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/002_DataTypes.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R8a6250edefca43e9"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataTypes" sheetId="1" r:id="R15759e0da4304bca"/>
   </x:sheets>
   <x:calcPr fullCalcOnLoad="1"/>
 </x:workbook>
@@ -97,7 +97,7 @@
         <x:v>Date:</x:v>
       </x:c>
       <x:c r="B4" s="2" t="n">
-        <x:v>46040.98596686342</x:v>
+        <x:v>46060.678136863426</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -105,7 +105,7 @@
         <x:v>DateTimeOffset:</x:v>
       </x:c>
       <x:c r="B5" s="2" t="n">
-        <x:v>46040.98596686342</x:v>
+        <x:v>46060.678136863426</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>